<commit_message>
most of the stuff is done, working
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Employees" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Projects" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Variables" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -118,6 +119,18 @@
   </si>
   <si>
     <t xml:space="preserve">Curvature Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of People per Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Working Hours Every Month</t>
   </si>
 </sst>
 </file>
@@ -132,6 +145,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,16 +205,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -283,10 +305,10 @@
       <c r="F2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H2" s="2" t="n">
+      <c r="G2" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -309,10 +331,10 @@
       <c r="F3" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H3" s="2" t="n">
+      <c r="G3" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -335,10 +357,10 @@
       <c r="F4" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H4" s="2" t="n">
+      <c r="G4" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -361,10 +383,10 @@
       <c r="F5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H5" s="2" t="n">
+      <c r="G5" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -387,10 +409,10 @@
       <c r="F6" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H6" s="2" t="n">
+      <c r="G6" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -413,10 +435,10 @@
       <c r="F7" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H7" s="2" t="n">
+      <c r="G7" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -439,10 +461,10 @@
       <c r="F8" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H8" s="2" t="n">
+      <c r="G8" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -465,10 +487,10 @@
       <c r="F9" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H9" s="2" t="n">
+      <c r="G9" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -491,10 +513,10 @@
       <c r="F10" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H10" s="2" t="n">
+      <c r="G10" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -517,10 +539,10 @@
       <c r="F11" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H11" s="2" t="n">
+      <c r="G11" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>72.3</v>
       </c>
     </row>
@@ -542,68 +564,68 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="38.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -631,47 +653,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="26.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="3" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>